<commit_message>
Updated with parallel execution. TO DO : Handle menu selection for multiple scenarios(need to handle flag).
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/MastekBlanketPOM/data/LeaveEntitlement.xlsx
+++ b/src/main/java/com/test/automation/MastekBlanketPOM/data/LeaveEntitlement.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Somesh\NewFrame\MastekBlanketPOM\src\main\java\com\test\automation\MastekBlanketPOM\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parth\git\MastekBlanketPOM\src\main\java\com\test\automation\MastekBlanketPOM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="LeaveEntitlement" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
   <si>
     <t>TestCase</t>
   </si>
@@ -74,9 +75,6 @@
     <t>Sales</t>
   </si>
   <si>
-    <t>Fiona Grace</t>
-  </si>
-  <si>
     <t>Maternity US</t>
   </si>
   <si>
@@ -89,10 +87,13 @@
     <t>2018-01-01 - 2018-12-31</t>
   </si>
   <si>
-    <t>Hannah Flores</t>
-  </si>
-  <si>
     <t>TC004</t>
+  </si>
+  <si>
+    <t>Fiona</t>
+  </si>
+  <si>
+    <t>Hannah</t>
   </si>
 </sst>
 </file>
@@ -410,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,13 +470,91 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
         <v>16</v>
       </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
       <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
         <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
       </c>
       <c r="I2">
         <v>12</v>
@@ -492,13 +571,13 @@
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
         <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
       </c>
       <c r="I3">
         <v>4</v>
@@ -521,10 +600,10 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
         <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
       </c>
       <c r="I4">
         <v>3</v>
@@ -535,19 +614,19 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
         <v>19</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
       </c>
       <c r="I5">
         <v>1</v>

</xml_diff>

<commit_message>
Updated : Extent report for parallel execution. To Do: 1. Add screenshot in report. 2. Add Log through listener. 3. create another thread and check report for parallel execution.
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/MastekBlanketPOM/data/LeaveEntitlement.xlsx
+++ b/src/main/java/com/test/automation/MastekBlanketPOM/data/LeaveEntitlement.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parth\git\MastekBlanketPOM\src\main\java\com\test\automation\MastekBlanketPOM\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Somesh\NewFrame\MastekBlanketPOM\src\main\java\com\test\automation\MastekBlanketPOM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="26">
   <si>
     <t>TestCase</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>Hannah</t>
+  </si>
+  <si>
+    <t>2016-01-01 - 2016-12-31</t>
+  </si>
+  <si>
+    <t>Russel</t>
+  </si>
+  <si>
+    <t>Thomas</t>
   </si>
 </sst>
 </file>
@@ -411,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,16 +479,88 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
         <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I2">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>